<commit_message>
important data cleaning update
</commit_message>
<xml_diff>
--- a/IRR_ols1.xlsx
+++ b/IRR_ols1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -38,6 +38,9 @@
     <t xml:space="preserve">poly(Fund_PIGHHI, 2)2</t>
   </si>
   <si>
+    <t xml:space="preserve">as.factor(Deal_Year)1981</t>
+  </si>
+  <si>
     <t xml:space="preserve">as.factor(Deal_Year)1982</t>
   </si>
   <si>
@@ -152,149 +155,182 @@
     <t xml:space="preserve">(1)</t>
   </si>
   <si>
-    <t xml:space="preserve">2.001 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.866)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.930)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.962 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.976)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.812 **</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.928)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1.044)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.900)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1.060)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1.059)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.546 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1.223)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.815 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.918)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.907)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.789 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.901)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.903)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.823 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.885)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.893)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.888)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.884)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.882)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.878)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.874)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.873)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.871)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.145 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.066 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.875)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.897 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.879)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.804 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.881)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.941 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.890)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.028 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.894)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.977 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.904 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.969)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.982 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.950)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.927)  </t>
+    <t xml:space="preserve">2.162 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.549)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.588)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.615)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.614)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.587)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.370 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.665)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.573)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.775)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.387 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.672)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.532 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.386 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.735 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.327 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.582)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.347 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.575)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.313 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.571)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.324 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.561)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.262 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.566)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.151 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.562)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.118 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.560)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.234 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.559)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.556)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.257 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.553)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.137 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.240 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.552)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.641 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.551)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.505 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.554)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.552 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.555)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.447 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.557)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.425 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.331 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.563)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.603 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.535 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.564)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.582 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.470 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.576)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.394 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.602)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.183 *  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="80">
+  <numFmts count="82">
     <numFmt numFmtId="50000" formatCode="0.000"/>
     <numFmt numFmtId="50001" formatCode="0.000"/>
     <numFmt numFmtId="50002" formatCode="0.000"/>
@@ -375,6 +411,8 @@
     <numFmt numFmtId="50077" formatCode="0.000"/>
     <numFmt numFmtId="50078" formatCode="0.000"/>
     <numFmt numFmtId="50079" formatCode="0.000"/>
+    <numFmt numFmtId="50080" formatCode="0.000"/>
+    <numFmt numFmtId="50081" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -480,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="center" vertical="top"/>
@@ -722,22 +760,28 @@
     <xf numFmtId="50074" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="50075" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="50075" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="0" horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="50076" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="0" horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="50077" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="50076" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="50077" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="50078" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="50079" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="50079" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="0" horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="50080" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="0" horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="50081" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1038,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">
@@ -1046,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
@@ -1054,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
@@ -1062,7 +1106,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="n">
-        <v>-0.426</v>
+        <v>0.203</v>
       </c>
     </row>
     <row r="5">
@@ -1070,15 +1114,15 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>49</v>
+      <c r="B6" s="10" t="n">
+        <v>0.957</v>
       </c>
     </row>
     <row r="7">
@@ -1093,8 +1137,8 @@
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>51</v>
+      <c r="B8" s="12" t="n">
+        <v>-0.843</v>
       </c>
     </row>
     <row r="9">
@@ -1102,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
@@ -1110,7 +1154,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="14" t="n">
-        <v>0.495</v>
+        <v>0.673</v>
       </c>
     </row>
     <row r="11">
@@ -1125,8 +1169,8 @@
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="16" t="n">
-        <v>0.018</v>
+      <c r="B12" s="16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13">
@@ -1134,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
@@ -1142,7 +1186,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="18" t="n">
-        <v>0.604</v>
+        <v>0.835</v>
       </c>
     </row>
     <row r="15">
@@ -1150,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16">
@@ -1158,7 +1202,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="20" t="n">
-        <v>-1.728</v>
+        <v>-1.177</v>
       </c>
     </row>
     <row r="17">
@@ -1166,15 +1210,15 @@
         <v>0</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="22" t="n">
-        <v>-2.01</v>
+      <c r="B18" s="22" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19">
@@ -1182,15 +1226,15 @@
         <v>0</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="24" t="n">
-        <v>-1.842</v>
+      <c r="B20" s="24" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="21">
@@ -1198,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22">
@@ -1206,7 +1250,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23">
@@ -1214,15 +1258,15 @@
         <v>0</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="28" t="n">
-        <v>-1.938</v>
+      <c r="B24" s="28" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25">
@@ -1237,8 +1281,8 @@
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="30" t="s">
-        <v>59</v>
+      <c r="B26" s="30" t="n">
+        <v>-1.438</v>
       </c>
     </row>
     <row r="27">
@@ -1246,15 +1290,15 @@
         <v>0</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="32" t="n">
-        <v>-1.755</v>
+      <c r="B28" s="32" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="29">
@@ -1262,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30">
@@ -1270,7 +1314,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31">
@@ -1278,15 +1322,15 @@
         <v>0</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="36" t="n">
-        <v>-1.425</v>
+      <c r="B32" s="36" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="33">
@@ -1294,15 +1338,15 @@
         <v>0</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="38" t="s">
-        <v>65</v>
+      <c r="B34" s="38" t="n">
+        <v>-1.069</v>
       </c>
     </row>
     <row r="35">
@@ -1310,15 +1354,15 @@
         <v>0</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="40" t="n">
-        <v>-1.697</v>
+      <c r="B36" s="40" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="37">
@@ -1326,15 +1370,15 @@
         <v>0</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="42" t="n">
-        <v>-1.634</v>
+      <c r="B38" s="42" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="39">
@@ -1342,15 +1386,15 @@
         <v>0</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="44" t="n">
-        <v>-1.495</v>
+      <c r="B40" s="44" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="41">
@@ -1358,15 +1402,15 @@
         <v>0</v>
       </c>
       <c r="B41" s="45" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="46" t="n">
-        <v>-1.626</v>
+      <c r="B42" s="46" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="43">
@@ -1374,15 +1418,15 @@
         <v>0</v>
       </c>
       <c r="B43" s="47" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="48" t="n">
-        <v>-1.578</v>
+      <c r="B44" s="48" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="45">
@@ -1390,15 +1434,15 @@
         <v>0</v>
       </c>
       <c r="B45" s="49" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="50" t="n">
-        <v>-1.498</v>
+      <c r="B46" s="50" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="47">
@@ -1406,15 +1450,15 @@
         <v>0</v>
       </c>
       <c r="B47" s="51" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="52" t="n">
-        <v>-1.457</v>
+      <c r="B48" s="52" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="49">
@@ -1422,15 +1466,15 @@
         <v>0</v>
       </c>
       <c r="B49" s="53" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="54" t="n">
-        <v>-1.476</v>
+      <c r="B50" s="54" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="51">
@@ -1438,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="B51" s="55" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52">
@@ -1446,7 +1490,7 @@
         <v>26</v>
       </c>
       <c r="B52" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53">
@@ -1454,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="B53" s="57" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54">
@@ -1462,7 +1506,7 @@
         <v>27</v>
       </c>
       <c r="B54" s="58" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55">
@@ -1470,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="B55" s="59" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56">
@@ -1478,7 +1522,7 @@
         <v>28</v>
       </c>
       <c r="B56" s="60" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57">
@@ -1486,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="B57" s="61" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58">
@@ -1494,7 +1538,7 @@
         <v>29</v>
       </c>
       <c r="B58" s="62" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59">
@@ -1502,15 +1546,15 @@
         <v>0</v>
       </c>
       <c r="B59" s="63" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B60" s="64" t="n">
-        <v>-1.6</v>
+      <c r="B60" s="64" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="61">
@@ -1518,15 +1562,15 @@
         <v>0</v>
       </c>
       <c r="B61" s="65" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="66" t="n">
-        <v>-1.69</v>
+      <c r="B62" s="66" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="63">
@@ -1534,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="B63" s="67" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64">
@@ -1542,7 +1586,7 @@
         <v>32</v>
       </c>
       <c r="B64" s="68" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65">
@@ -1550,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="B65" s="69" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66">
@@ -1558,7 +1602,7 @@
         <v>33</v>
       </c>
       <c r="B66" s="70" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67">
@@ -1566,15 +1610,15 @@
         <v>0</v>
       </c>
       <c r="B67" s="71" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B68" s="72" t="n">
-        <v>-1.758</v>
+      <c r="B68" s="72" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="69">
@@ -1582,7 +1626,7 @@
         <v>0</v>
       </c>
       <c r="B69" s="73" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70">
@@ -1590,7 +1634,7 @@
         <v>35</v>
       </c>
       <c r="B70" s="74" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71">
@@ -1598,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="B71" s="75" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72">
@@ -1606,7 +1650,7 @@
         <v>36</v>
       </c>
       <c r="B72" s="76" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73">
@@ -1614,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="B73" s="77" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74">
@@ -1622,7 +1666,7 @@
         <v>37</v>
       </c>
       <c r="B74" s="78" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75">
@@ -1630,15 +1674,15 @@
         <v>0</v>
       </c>
       <c r="B75" s="79" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="80" t="n">
-        <v>-1.608</v>
+      <c r="B76" s="80" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="77">
@@ -1646,58 +1690,74 @@
         <v>0</v>
       </c>
       <c r="B77" s="81" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B78" s="82" t="n">
-        <v>764</v>
+      <c r="B78" s="82" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B79" s="83" t="n">
-        <v>0.103</v>
+        <v>0</v>
+      </c>
+      <c r="B79" s="83" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B80" s="84" t="n">
-        <v>0.058</v>
+        <v>910</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B81" s="85" t="n">
+        <v>0.121</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B81" s="85" t="n">
-        <v>2.265</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="3" t="s">
+      <c r="B82" s="86" t="n">
+        <v>0.082</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B82" s="86" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="4" t="s">
+      <c r="B83" s="87" t="n">
+        <v>3.142</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B83" s="4"/>
+      <c r="B84" s="88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B85" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A85:B85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>